<commit_message>
Logout button and basic registration test
'python manage.py test'
</commit_message>
<xml_diff>
--- a/artefacts/Burndown Chart.xlsx
+++ b/artefacts/Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Harry/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Harry/Documents/Stop Over/Music/23rd of aug/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -229,7 +229,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -242,9 +242,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Actual Tasks Remaining</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -271,10 +268,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$E$13</c:f>
+              <c:f>Sheet1!$E$8:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -292,33 +289,63 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$8:$F$13</c:f>
+              <c:f>Sheet1!$F$8:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.0</c:v>
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,11 +360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2084819504"/>
-        <c:axId val="-2085453584"/>
+        <c:axId val="-2118847200"/>
+        <c:axId val="-2124740272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2084819504"/>
+        <c:axId val="-2118847200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20.0"/>
@@ -419,6 +446,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -455,15 +483,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085453584"/>
+        <c:crossAx val="-2124740272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2085453584"/>
+        <c:axId val="-2124740272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16.0"/>
+          <c:max val="35.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -579,7 +607,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084819504"/>
+        <c:crossAx val="-2118847200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1529,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1551,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="5:6" x14ac:dyDescent="0.2">
@@ -1567,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="5:6" x14ac:dyDescent="0.2">
@@ -1575,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="5:6" x14ac:dyDescent="0.2">
@@ -1583,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.2">
@@ -1591,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="F11">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="5:6" x14ac:dyDescent="0.2">
@@ -1599,7 +1627,7 @@
         <v>4</v>
       </c>
       <c r="F12">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="5:6" x14ac:dyDescent="0.2">
@@ -1607,7 +1635,47 @@
         <v>5</v>
       </c>
       <c r="F13">
-        <v>14</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.2">

</xml_diff>